<commit_message>
aggregate discrete range test
</commit_message>
<xml_diff>
--- a/tests/testMaterials/testForDiscreteRange/SparseMatricesForDiscreteRangeTest_2021_2022.xlsx
+++ b/tests/testMaterials/testForDiscreteRange/SparseMatricesForDiscreteRangeTest_2021_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\tests\testMaterials\testForDiscreteRange\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\RHIT_IRPA_@\rhit_IRPA_2023\tests\testMaterials\testForDiscreteRange\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8483B339-E55C-477E-B491-D1D9005BAEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EB852B-A443-4EC6-B9D2-641052E9309A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="act score_fake" sheetId="13" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t>Value</t>
   </si>
@@ -33,19 +33,49 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Operation-Allowed?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Sum-Allowed?</t>
+  </si>
+  <si>
+    <t>Range-Allowed?</t>
+  </si>
+  <si>
+    <t>Percentage-Allowed?</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -68,8 +98,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,13 +420,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F512CCB7-1852-4B4C-BFAD-2B89D373625B}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
     <col min="5" max="5" width="9.33203125" customWidth="1"/>
   </cols>
@@ -661,6 +697,46 @@
       </c>
       <c r="L7">
         <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -675,14 +751,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBAD6F5E-0B89-4DAA-97DC-F0A734D6F4E6}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -952,6 +1030,46 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>